<commit_message>
Added assessment for AZ-600 (beta)
</commit_message>
<xml_diff>
--- a/Assessments/Exam-Msft-PL-100-Self-Assessment-TheCloud42.xlsx
+++ b/Assessments/Exam-Msft-PL-100-Self-Assessment-TheCloud42.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RolfMcLaughl_cqz\Documents\GitHub\Assessment-Sheets\Assessments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15915408-D1AA-4C6B-9CEF-9199D55EBEE2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9AE4951-B922-434E-BC75-48A821E941EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3516" yWindow="1308" windowWidth="34560" windowHeight="13644" xr2:uid="{C935EA29-66AB-47BC-AD6E-3C33C43244A1}"/>
+    <workbookView xWindow="3864" yWindow="1656" windowWidth="34560" windowHeight="13644" xr2:uid="{C935EA29-66AB-47BC-AD6E-3C33C43244A1}"/>
   </bookViews>
   <sheets>
     <sheet name="Assessment Overview" sheetId="3" r:id="rId1"/>
@@ -145,9 +145,6 @@
     <t>https://github.com/TheCloud42/Assessment-Sheets</t>
   </si>
   <si>
-    <t>Microsoft Certified: Microsoft Power Platform App Maker Associate</t>
-  </si>
-  <si>
     <t>Design solutions (10-15%)</t>
   </si>
   <si>
@@ -514,6 +511,9 @@
   </si>
   <si>
     <t>Self Assessment last updated January 04, 2021</t>
+  </si>
+  <si>
+    <t>Exam PL-100: Microsoft Power Platform App Maker</t>
   </si>
 </sst>
 </file>
@@ -757,337 +757,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{53131793-09E6-461C-8EFA-0A1B2AF0414A}"/>
   </cellStyles>
-  <dxfs count="120">
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="87">
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -2270,7 +1940,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53880D26-65BA-4615-AC6E-5E99075537E5}">
   <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2328,12 +2000,12 @@
     </row>
     <row r="12" spans="1:2" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A12" s="9" t="s">
-        <v>36</v>
+        <v>155</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -2346,7 +2018,7 @@
     </row>
     <row r="16" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A16" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B16" s="13">
         <f>'Self Assessment'!D2</f>
@@ -2355,7 +2027,7 @@
     </row>
     <row r="17" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A17" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B17" s="13">
         <f>'Self Assessment'!D39</f>
@@ -2364,7 +2036,7 @@
     </row>
     <row r="18" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A18" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B18" s="13">
         <f>'Self Assessment'!D83</f>
@@ -2373,7 +2045,7 @@
     </row>
     <row r="19" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A19" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B19" s="13">
         <f>'Self Assessment'!D96</f>
@@ -2385,7 +2057,7 @@
         <v>14</v>
       </c>
       <c r="B20" s="11">
-        <f>SUM(B16:B19)/5</f>
+        <f>SUM(B16:B19)/4</f>
         <v>0</v>
       </c>
     </row>
@@ -2455,38 +2127,38 @@
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B16:B19">
-    <cfRule type="cellIs" dxfId="119" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="86" priority="9" operator="greaterThan">
       <formula>0.7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:B19">
-    <cfRule type="cellIs" dxfId="118" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="85" priority="8" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:B19">
-    <cfRule type="cellIs" dxfId="117" priority="7" operator="between">
+    <cfRule type="cellIs" dxfId="84" priority="7" operator="between">
       <formula>0.5</formula>
       <formula>0.7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20">
-    <cfRule type="cellIs" dxfId="116" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="83" priority="6" operator="greaterThan">
       <formula>0.7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20">
-    <cfRule type="cellIs" dxfId="115" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="82" priority="5" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20">
-    <cfRule type="cellIs" dxfId="114" priority="4" operator="between">
+    <cfRule type="cellIs" dxfId="81" priority="4" operator="between">
       <formula>0.5</formula>
       <formula>0.7</formula>
     </cfRule>
@@ -2537,7 +2209,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" s="26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D2" s="22">
         <f>SUM(D3,D9,D17,D22,D27,D31,D34)/E2</f>
@@ -2550,7 +2222,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B3" s="25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D3" s="23">
         <f>SUM(E4:E8)/E3</f>
@@ -2563,19 +2235,19 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="C4" s="27" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D4" t="s">
         <v>3</v>
       </c>
       <c r="E4" s="1">
-        <f t="shared" ref="E4:E27" si="0">IF(D4="Know Well",1,IF(D4="Know a Little",0.5,0))</f>
+        <f t="shared" ref="E4:E26" si="0">IF(D4="Know Well",1,IF(D4="Know a Little",0.5,0))</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="C5" s="27" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D5" t="s">
         <v>3</v>
@@ -2587,7 +2259,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="C6" s="27" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D6" t="s">
         <v>3</v>
@@ -2599,7 +2271,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.4">
       <c r="C7" s="27" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D7" t="s">
         <v>3</v>
@@ -2611,7 +2283,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.4">
       <c r="C8" s="27" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D8" t="s">
         <v>3</v>
@@ -2623,7 +2295,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B9" s="25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C9" s="27"/>
       <c r="D9" s="23">
@@ -2637,7 +2309,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="C10" s="27" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D10" t="s">
         <v>3</v>
@@ -2649,7 +2321,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="C11" s="27" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D11" t="s">
         <v>3</v>
@@ -2661,7 +2333,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="C12" s="27" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D12" t="s">
         <v>3</v>
@@ -2673,7 +2345,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.4">
       <c r="C13" s="27" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D13" t="s">
         <v>3</v>
@@ -2685,7 +2357,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.4">
       <c r="C14" s="27" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D14" t="s">
         <v>3</v>
@@ -2697,7 +2369,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.4">
       <c r="C15" s="27" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D15" t="s">
         <v>3</v>
@@ -2709,7 +2381,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.4">
       <c r="C16" s="27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D16" t="s">
         <v>3</v>
@@ -2721,7 +2393,7 @@
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B17" s="25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C17" s="27"/>
       <c r="D17" s="23">
@@ -2735,7 +2407,7 @@
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C18" s="27" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D18" t="s">
         <v>3</v>
@@ -2747,7 +2419,7 @@
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C19" s="27" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D19" t="s">
         <v>3</v>
@@ -2759,7 +2431,7 @@
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C20" s="27" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D20" t="s">
         <v>3</v>
@@ -2771,7 +2443,7 @@
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C21" s="27" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D21" t="s">
         <v>3</v>
@@ -2783,7 +2455,7 @@
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B22" s="25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C22" s="27"/>
       <c r="D22" s="23">
@@ -2797,7 +2469,7 @@
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C23" s="27" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D23" t="s">
         <v>3</v>
@@ -2809,7 +2481,7 @@
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C24" s="27" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D24" t="s">
         <v>3</v>
@@ -2821,7 +2493,7 @@
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C25" s="27" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D25" t="s">
         <v>3</v>
@@ -2833,7 +2505,7 @@
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C26" s="27" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D26" t="s">
         <v>3</v>
@@ -2845,7 +2517,7 @@
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B27" s="25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C27" s="27"/>
       <c r="D27" s="23">
@@ -2859,7 +2531,7 @@
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C28" s="27" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D28" t="s">
         <v>3</v>
@@ -2871,7 +2543,7 @@
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C29" s="27" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D29" t="s">
         <v>3</v>
@@ -2883,7 +2555,7 @@
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C30" s="27" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D30" t="s">
         <v>3</v>
@@ -2895,7 +2567,7 @@
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B31" s="25" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C31" s="27"/>
       <c r="D31" s="23">
@@ -2909,7 +2581,7 @@
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C32" s="27" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D32" t="s">
         <v>3</v>
@@ -2921,7 +2593,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.4">
       <c r="C33" s="27" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D33" t="s">
         <v>3</v>
@@ -2933,7 +2605,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B34" s="25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C34" s="27"/>
       <c r="D34" s="23">
@@ -2947,7 +2619,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.4">
       <c r="C35" s="27" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D35" t="s">
         <v>3</v>
@@ -2959,7 +2631,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.4">
       <c r="C36" s="27" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D36" t="s">
         <v>3</v>
@@ -2971,7 +2643,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.4">
       <c r="C37" s="27" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D37" t="s">
         <v>3</v>
@@ -2983,7 +2655,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.4">
       <c r="C38" s="27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D38" t="s">
         <v>3</v>
@@ -2995,7 +2667,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A39" s="24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C39" s="27"/>
       <c r="D39" s="22">
@@ -3009,7 +2681,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B40" s="25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C40" s="27"/>
       <c r="D40" s="23">
@@ -3023,7 +2695,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.4">
       <c r="C41" s="27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D41" t="s">
         <v>3</v>
@@ -3035,7 +2707,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.4">
       <c r="C42" s="27" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D42" t="s">
         <v>3</v>
@@ -3047,7 +2719,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.4">
       <c r="C43" s="27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D43" t="s">
         <v>3</v>
@@ -3073,7 +2745,7 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.4">
       <c r="C45" s="27" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D45" t="s">
         <v>3</v>
@@ -3085,7 +2757,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.4">
       <c r="C46" s="27" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D46" t="s">
         <v>3</v>
@@ -3097,7 +2769,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.4">
       <c r="C47" s="27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D47" t="s">
         <v>3</v>
@@ -3109,7 +2781,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.4">
       <c r="C48" s="27" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D48" t="s">
         <v>3</v>
@@ -3121,7 +2793,7 @@
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C49" s="27" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D49" t="s">
         <v>3</v>
@@ -3147,103 +2819,103 @@
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C51" s="27" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D51" t="s">
         <v>3</v>
       </c>
       <c r="E51" s="1">
-        <f>IF(D51="Know Well",1,IF(D51="Know a Little",0.5,0))</f>
+        <f t="shared" ref="E51:E58" si="3">IF(D51="Know Well",1,IF(D51="Know a Little",0.5,0))</f>
         <v>0</v>
       </c>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C52" s="27" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D52" t="s">
         <v>3</v>
       </c>
       <c r="E52" s="1">
-        <f>IF(D52="Know Well",1,IF(D52="Know a Little",0.5,0))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C53" s="27" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D53" t="s">
         <v>3</v>
       </c>
       <c r="E53" s="1">
-        <f>IF(D53="Know Well",1,IF(D53="Know a Little",0.5,0))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C54" s="27" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D54" t="s">
         <v>3</v>
       </c>
       <c r="E54" s="1">
-        <f>IF(D54="Know Well",1,IF(D54="Know a Little",0.5,0))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C55" s="27" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D55" t="s">
         <v>3</v>
       </c>
       <c r="E55" s="1">
-        <f>IF(D55="Know Well",1,IF(D55="Know a Little",0.5,0))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C56" s="27" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D56" t="s">
         <v>3</v>
       </c>
       <c r="E56" s="1">
-        <f>IF(D56="Know Well",1,IF(D56="Know a Little",0.5,0))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C57" s="27" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D57" t="s">
         <v>3</v>
       </c>
       <c r="E57" s="1">
-        <f>IF(D57="Know Well",1,IF(D57="Know a Little",0.5,0))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C58" s="27" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D58" t="s">
         <v>3</v>
       </c>
       <c r="E58" s="1">
-        <f>IF(D58="Know Well",1,IF(D58="Know a Little",0.5,0))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B59" s="25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C59" s="27"/>
       <c r="D59" s="23">
@@ -3257,7 +2929,7 @@
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C60" s="27" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D60" t="s">
         <v>3</v>
@@ -3269,7 +2941,7 @@
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C61" s="27" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D61" t="s">
         <v>3</v>
@@ -3281,7 +2953,7 @@
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B62" s="25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C62" s="27"/>
       <c r="D62" s="23">
@@ -3295,7 +2967,7 @@
     </row>
     <row r="63" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C63" s="27" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D63" t="s">
         <v>3</v>
@@ -3307,7 +2979,7 @@
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C64" s="27" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D64" t="s">
         <v>3</v>
@@ -3319,7 +2991,7 @@
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C65" s="27" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D65" t="s">
         <v>3</v>
@@ -3331,7 +3003,7 @@
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C66" s="27" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D66" t="s">
         <v>3</v>
@@ -3343,7 +3015,7 @@
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C67" s="27" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D67" t="s">
         <v>3</v>
@@ -3355,7 +3027,7 @@
     </row>
     <row r="68" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B68" s="25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C68" s="27"/>
       <c r="D68" s="23">
@@ -3369,7 +3041,7 @@
     </row>
     <row r="69" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C69" s="27" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D69" t="s">
         <v>3</v>
@@ -3381,7 +3053,7 @@
     </row>
     <row r="70" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C70" s="27" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D70" t="s">
         <v>3</v>
@@ -3393,7 +3065,7 @@
     </row>
     <row r="71" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C71" s="27" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D71" t="s">
         <v>3</v>
@@ -3405,7 +3077,7 @@
     </row>
     <row r="72" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C72" s="27" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D72" t="s">
         <v>3</v>
@@ -3417,7 +3089,7 @@
     </row>
     <row r="73" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C73" s="27" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D73" t="s">
         <v>3</v>
@@ -3429,7 +3101,7 @@
     </row>
     <row r="74" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B74" s="25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C74" s="27"/>
       <c r="D74" s="23">
@@ -3443,7 +3115,7 @@
     </row>
     <row r="75" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C75" s="27" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D75" t="s">
         <v>3</v>
@@ -3455,7 +3127,7 @@
     </row>
     <row r="76" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C76" s="27" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D76" t="s">
         <v>3</v>
@@ -3467,7 +3139,7 @@
     </row>
     <row r="77" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C77" s="27" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D77" t="s">
         <v>3</v>
@@ -3479,7 +3151,7 @@
     </row>
     <row r="78" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C78" s="27" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D78" t="s">
         <v>3</v>
@@ -3491,55 +3163,55 @@
     </row>
     <row r="79" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C79" s="27" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D79" t="s">
         <v>3</v>
       </c>
       <c r="E79" s="1">
-        <f t="shared" ref="E79:E127" si="3">IF(D79="Know Well",1,IF(D79="Know a Little",0.5,0))</f>
+        <f t="shared" ref="E79:E95" si="4">IF(D79="Know Well",1,IF(D79="Know a Little",0.5,0))</f>
         <v>0</v>
       </c>
     </row>
     <row r="80" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C80" s="27" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D80" t="s">
         <v>3</v>
       </c>
       <c r="E80" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.4">
       <c r="C81" s="27" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D81" t="s">
         <v>3</v>
       </c>
       <c r="E81" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.4">
       <c r="C82" s="27" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D82" t="s">
         <v>3</v>
       </c>
       <c r="E82" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A83" s="24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B83" s="25"/>
       <c r="C83" s="27"/>
@@ -3554,7 +3226,7 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B84" s="25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C84" s="27"/>
       <c r="D84" s="23">
@@ -3568,31 +3240,31 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.4">
       <c r="C85" s="27" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D85" t="s">
         <v>3</v>
       </c>
       <c r="E85" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.4">
       <c r="C86" s="27" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D86" t="s">
         <v>3</v>
       </c>
       <c r="E86" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B87" s="25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C87" s="27"/>
       <c r="D87" s="23">
@@ -3606,55 +3278,55 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.4">
       <c r="C88" s="27" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D88" t="s">
         <v>3</v>
       </c>
       <c r="E88" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.4">
       <c r="C89" s="27" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D89" t="s">
         <v>3</v>
       </c>
       <c r="E89" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.4">
       <c r="C90" s="27" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D90" t="s">
         <v>3</v>
       </c>
       <c r="E90" s="1">
-        <f t="shared" ref="E90" si="4">IF(D90="Know Well",1,IF(D90="Know a Little",0.5,0))</f>
+        <f t="shared" ref="E90" si="5">IF(D90="Know Well",1,IF(D90="Know a Little",0.5,0))</f>
         <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.4">
       <c r="C91" s="27" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D91" t="s">
         <v>3</v>
       </c>
       <c r="E91" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B92" s="25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C92" s="27"/>
       <c r="D92" s="23">
@@ -3668,43 +3340,43 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.4">
       <c r="C93" s="27" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D93" t="s">
         <v>3</v>
       </c>
       <c r="E93" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.4">
       <c r="C94" s="27" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D94" t="s">
         <v>3</v>
       </c>
       <c r="E94" s="1">
-        <f t="shared" ref="E94" si="5">IF(D94="Know Well",1,IF(D94="Know a Little",0.5,0))</f>
+        <f t="shared" ref="E94" si="6">IF(D94="Know Well",1,IF(D94="Know a Little",0.5,0))</f>
         <v>0</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.4">
       <c r="C95" s="27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D95" t="s">
         <v>3</v>
       </c>
       <c r="E95" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A96" s="24" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C96" s="27"/>
       <c r="D96" s="22">
@@ -3718,7 +3390,7 @@
     </row>
     <row r="97" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B97" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C97" s="27"/>
       <c r="D97" s="23">
@@ -3732,7 +3404,7 @@
     </row>
     <row r="98" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C98" s="27" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D98" t="s">
         <v>3</v>
@@ -3744,7 +3416,7 @@
     </row>
     <row r="99" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C99" s="27" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D99" t="s">
         <v>3</v>
@@ -3756,7 +3428,7 @@
     </row>
     <row r="100" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B100" s="25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C100" s="27"/>
       <c r="D100" s="23">
@@ -3770,7 +3442,7 @@
     </row>
     <row r="101" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C101" s="27" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D101" t="s">
         <v>3</v>
@@ -3782,7 +3454,7 @@
     </row>
     <row r="102" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C102" s="27" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D102" t="s">
         <v>3</v>
@@ -3794,7 +3466,7 @@
     </row>
     <row r="103" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C103" s="27" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D103" t="s">
         <v>3</v>
@@ -3806,7 +3478,7 @@
     </row>
     <row r="104" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B104" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C104" s="27"/>
       <c r="D104" s="23">
@@ -3820,7 +3492,7 @@
     </row>
     <row r="105" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C105" s="27" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D105" t="s">
         <v>3</v>
@@ -3832,43 +3504,43 @@
     </row>
     <row r="106" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C106" s="27" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D106" t="s">
         <v>3</v>
       </c>
       <c r="E106" s="1">
-        <f t="shared" ref="E106:E116" si="6">IF(D106="Know Well",1,IF(D106="Know a Little",0.5,0))</f>
+        <f t="shared" ref="E106:E116" si="7">IF(D106="Know Well",1,IF(D106="Know a Little",0.5,0))</f>
         <v>0</v>
       </c>
     </row>
     <row r="107" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C107" s="27" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D107" t="s">
         <v>3</v>
       </c>
       <c r="E107" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="108" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C108" s="27" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D108" t="s">
         <v>3</v>
       </c>
       <c r="E108" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="109" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B109" s="25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C109" s="27"/>
       <c r="D109" s="23">
@@ -3882,43 +3554,43 @@
     </row>
     <row r="110" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C110" s="27" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D110" t="s">
         <v>3</v>
       </c>
       <c r="E110" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="111" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C111" s="27" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D111" t="s">
         <v>3</v>
       </c>
       <c r="E111" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="112" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C112" s="27" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D112" t="s">
         <v>3</v>
       </c>
       <c r="E112" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="113" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B113" s="25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C113" s="27"/>
       <c r="D113" s="23">
@@ -3932,180 +3604,180 @@
     </row>
     <row r="114" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C114" s="27" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D114" t="s">
         <v>3</v>
       </c>
       <c r="E114" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="115" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C115" s="27" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D115" t="s">
         <v>3</v>
       </c>
       <c r="E115" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="116" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C116" s="27" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D116" t="s">
         <v>3</v>
       </c>
       <c r="E116" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D4:D8 D18:D21 D41:D43 D23:D26 D28:D30 D32:D33 D35:D38 D10:D16 D51:D58 D60:D61 D45:D49 D63:D67 D69:D73 D75:D82 D85:D86 D88:D91 D93:D95 D98:D99 D101:D103 D105:D108 D110:D112 D114:D116">
-    <cfRule type="cellIs" dxfId="113" priority="375" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="375" operator="equal">
       <formula>"No Idea"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:D8 D18:D21 D41:D43 D23:D26 D28:D30 D32:D33 D35:D38 D10:D16 D51:D58 D60:D61 D45:D49 D63:D67 D69:D73 D75:D82 D85:D86 D88:D91 D93:D95 D98:D99 D101:D103 D105:D108 D110:D112 D114:D116">
-    <cfRule type="cellIs" dxfId="112" priority="374" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="374" operator="equal">
       <formula>"Know a Little"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:D8 D18:D21 D41:D43 D23:D26 D28:D30 D32:D33 D35:D38 D10:D16 D51:D58 D60:D61 D45:D49 D63:D67 D69:D73 D75:D82 D85:D86 D88:D91 D93:D95 D98:D99 D101:D103 D105:D108 D110:D112 D114:D116">
-    <cfRule type="cellIs" dxfId="111" priority="373" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="373" operator="equal">
       <formula>"Know Well"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="110" priority="309" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="77" priority="309" operator="greaterThan">
       <formula>0.7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="109" priority="308" operator="lessThan">
+    <cfRule type="cellIs" dxfId="76" priority="308" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="108" priority="307" operator="between">
+    <cfRule type="cellIs" dxfId="75" priority="307" operator="between">
       <formula>0.5</formula>
       <formula>0.7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="cellIs" dxfId="107" priority="312" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="74" priority="312" operator="greaterThan">
       <formula>0.7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="cellIs" dxfId="106" priority="311" operator="lessThan">
+    <cfRule type="cellIs" dxfId="73" priority="311" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="cellIs" dxfId="105" priority="310" operator="between">
+    <cfRule type="cellIs" dxfId="72" priority="310" operator="between">
       <formula>0.5</formula>
       <formula>0.7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D17">
-    <cfRule type="cellIs" dxfId="101" priority="102" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="71" priority="102" operator="greaterThan">
       <formula>0.7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D17">
-    <cfRule type="cellIs" dxfId="100" priority="101" operator="lessThan">
+    <cfRule type="cellIs" dxfId="70" priority="101" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D17">
-    <cfRule type="cellIs" dxfId="99" priority="100" operator="between">
+    <cfRule type="cellIs" dxfId="69" priority="100" operator="between">
       <formula>0.5</formula>
       <formula>0.7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D22">
-    <cfRule type="cellIs" dxfId="98" priority="99" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="68" priority="99" operator="greaterThan">
       <formula>0.7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D22">
-    <cfRule type="cellIs" dxfId="97" priority="98" operator="lessThan">
+    <cfRule type="cellIs" dxfId="67" priority="98" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D22">
-    <cfRule type="cellIs" dxfId="96" priority="97" operator="between">
+    <cfRule type="cellIs" dxfId="66" priority="97" operator="between">
       <formula>0.5</formula>
       <formula>0.7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D40">
-    <cfRule type="cellIs" dxfId="95" priority="96" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="65" priority="96" operator="greaterThan">
       <formula>0.7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D40">
-    <cfRule type="cellIs" dxfId="94" priority="95" operator="lessThan">
+    <cfRule type="cellIs" dxfId="64" priority="95" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D40">
-    <cfRule type="cellIs" dxfId="93" priority="94" operator="between">
+    <cfRule type="cellIs" dxfId="63" priority="94" operator="between">
       <formula>0.5</formula>
       <formula>0.7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D84">
-    <cfRule type="cellIs" dxfId="77" priority="78" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="62" priority="78" operator="greaterThan">
       <formula>0.7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D84">
-    <cfRule type="cellIs" dxfId="76" priority="77" operator="lessThan">
+    <cfRule type="cellIs" dxfId="61" priority="77" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D84">
-    <cfRule type="cellIs" dxfId="75" priority="76" operator="between">
+    <cfRule type="cellIs" dxfId="60" priority="76" operator="between">
       <formula>0.5</formula>
       <formula>0.7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D97">
-    <cfRule type="cellIs" dxfId="68" priority="69" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="59" priority="69" operator="greaterThan">
       <formula>0.7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D97">
-    <cfRule type="cellIs" dxfId="67" priority="68" operator="lessThan">
+    <cfRule type="cellIs" dxfId="58" priority="68" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D97">
-    <cfRule type="cellIs" dxfId="66" priority="67" operator="between">
+    <cfRule type="cellIs" dxfId="57" priority="67" operator="between">
       <formula>0.5</formula>
       <formula>0.7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D39">
-    <cfRule type="cellIs" dxfId="59" priority="60" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="56" priority="60" operator="greaterThan">
       <formula>0.7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D39">
-    <cfRule type="cellIs" dxfId="58" priority="59" operator="lessThan">
+    <cfRule type="cellIs" dxfId="55" priority="59" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D39">
-    <cfRule type="cellIs" dxfId="57" priority="58" operator="between">
+    <cfRule type="cellIs" dxfId="54" priority="58" operator="between">
       <formula>0.5</formula>
       <formula>0.7</formula>
     </cfRule>
@@ -4453,6 +4125,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EF07142713CD6D4C83CBD8BC01D705B5" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="32aeae619b2d68ad0a0a617232c5ed1c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns3="fdf91ed2-bd70-42ba-ab71-fba0383985f7" xmlns:ns4="f0622a8f-13ca-4d7c-a754-eaa399ac8b4a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3241b21036c9de17defa365b42b3bf51" ns1:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -4692,15 +4373,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -4711,6 +4383,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F35C236B-8AE1-436F-B1E2-ED8D2060C8FD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4EDD4A3B-2670-4E44-82A3-4A8CB7637D80}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4730,14 +4410,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F35C236B-8AE1-436F-B1E2-ED8D2060C8FD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D59C97D4-D35A-4BE7-99D7-230B389AC139}">
   <ds:schemaRefs>

</xml_diff>